<commit_message>
Added sequential data experiments
</commit_message>
<xml_diff>
--- a/key_value_storage/measurements/results/StableRBTree.xlsx
+++ b/key_value_storage/measurements/results/StableRBTree.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="128">
   <si>
     <t/>
   </si>
@@ -70,172 +70,169 @@
     <t>Δ Allocated memory</t>
   </si>
   <si>
-    <t>268</t>
-  </si>
-  <si>
-    <t>3508</t>
-  </si>
-  <si>
-    <t>59608</t>
-  </si>
-  <si>
-    <t>891496</t>
-  </si>
-  <si>
-    <t>11854600</t>
-  </si>
-  <si>
-    <t>148638472</t>
-  </si>
-  <si>
-    <t>1786186564</t>
+    <t>104</t>
+  </si>
+  <si>
+    <t>2960</t>
+  </si>
+  <si>
+    <t>58892</t>
+  </si>
+  <si>
+    <t>890420</t>
+  </si>
+  <si>
+    <t>11853344</t>
+  </si>
+  <si>
+    <t>148636976</t>
+  </si>
+  <si>
+    <t>1786184828</t>
   </si>
   <si>
     <t>Δ Reclaimed memory</t>
   </si>
   <si>
-    <t>164</t>
-  </si>
-  <si>
-    <t>2936</t>
-  </si>
-  <si>
-    <t>54356</t>
-  </si>
-  <si>
-    <t>839444</t>
-  </si>
-  <si>
-    <t>11334548</t>
-  </si>
-  <si>
-    <t>143438420</t>
-  </si>
-  <si>
-    <t>1734186476</t>
+    <t>52</t>
+  </si>
+  <si>
+    <t>2440</t>
+  </si>
+  <si>
+    <t>53692</t>
+  </si>
+  <si>
+    <t>838420</t>
+  </si>
+  <si>
+    <t>11333344</t>
+  </si>
+  <si>
+    <t>143436976</t>
+  </si>
+  <si>
+    <t>1734184792</t>
   </si>
   <si>
     <t>Δ Heap memory</t>
   </si>
   <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>572</t>
-  </si>
-  <si>
-    <t>5252</t>
-  </si>
-  <si>
-    <t>52052</t>
-  </si>
-  <si>
-    <t>520052</t>
-  </si>
-  <si>
-    <t>5200052</t>
-  </si>
-  <si>
-    <t>52000160</t>
+    <t>520</t>
+  </si>
+  <si>
+    <t>5200</t>
+  </si>
+  <si>
+    <t>52000</t>
+  </si>
+  <si>
+    <t>520000</t>
+  </si>
+  <si>
+    <t>5200000</t>
+  </si>
+  <si>
+    <t>52000108</t>
   </si>
   <si>
     <t>Δ Instructions</t>
   </si>
   <si>
-    <t>1011</t>
-  </si>
-  <si>
-    <t>16245</t>
-  </si>
-  <si>
-    <t>316409</t>
-  </si>
-  <si>
-    <t>5033929</t>
-  </si>
-  <si>
-    <t>69163189</t>
-  </si>
-  <si>
-    <t>884146395</t>
-  </si>
-  <si>
-    <t>10757631571</t>
+    <t>305</t>
+  </si>
+  <si>
+    <t>13754</t>
+  </si>
+  <si>
+    <t>312504</t>
+  </si>
+  <si>
+    <t>5027762</t>
+  </si>
+  <si>
+    <t>69155791</t>
+  </si>
+  <si>
+    <t>884137449</t>
+  </si>
+  <si>
+    <t>10757621077</t>
   </si>
   <si>
     <t>Δ GC instructions</t>
   </si>
   <si>
-    <t>2222</t>
-  </si>
-  <si>
-    <t>12199</t>
-  </si>
-  <si>
-    <t>111917</t>
-  </si>
-  <si>
-    <t>1109485</t>
-  </si>
-  <si>
-    <t>11084061</t>
-  </si>
-  <si>
-    <t>110830557</t>
-  </si>
-  <si>
-    <t>1108293309</t>
+    <t>1117</t>
+  </si>
+  <si>
+    <t>11086</t>
+  </si>
+  <si>
+    <t>110804</t>
+  </si>
+  <si>
+    <t>1108372</t>
+  </si>
+  <si>
+    <t>11082948</t>
+  </si>
+  <si>
+    <t>110829444</t>
+  </si>
+  <si>
+    <t>1108292196</t>
   </si>
   <si>
     <t>Δ Mutator instructions</t>
   </si>
   <si>
-    <t>7194</t>
-  </si>
-  <si>
-    <t>23490</t>
-  </si>
-  <si>
-    <t>334274</t>
-  </si>
-  <si>
-    <t>5158015</t>
-  </si>
-  <si>
-    <t>70349275</t>
-  </si>
-  <si>
-    <t>895952502</t>
-  </si>
-  <si>
-    <t>10875637710</t>
+    <t>6411</t>
+  </si>
+  <si>
+    <t>20922</t>
+  </si>
+  <si>
+    <t>330292</t>
+  </si>
+  <si>
+    <t>5151771</t>
+  </si>
+  <si>
+    <t>70341800</t>
+  </si>
+  <si>
+    <t>895943479</t>
+  </si>
+  <si>
+    <t>10875627139</t>
   </si>
   <si>
     <t>24</t>
   </si>
   <si>
-    <t>417</t>
-  </si>
-  <si>
-    <t>4125</t>
-  </si>
-  <si>
-    <t>71515</t>
-  </si>
-  <si>
-    <t>1117591</t>
-  </si>
-  <si>
-    <t>14542209</t>
-  </si>
-  <si>
-    <t>181408457</t>
-  </si>
-  <si>
-    <t>2229655521</t>
-  </si>
-  <si>
-    <t>450000045</t>
+    <t>141</t>
+  </si>
+  <si>
+    <t>3846</t>
+  </si>
+  <si>
+    <t>70338</t>
+  </si>
+  <si>
+    <t>1115604</t>
+  </si>
+  <si>
+    <t>14539817</t>
+  </si>
+  <si>
+    <t>181405525</t>
+  </si>
+  <si>
+    <t>2229652049</t>
+  </si>
+  <si>
+    <t>450000000</t>
   </si>
   <si>
     <t>-368</t>
@@ -250,160 +247,157 @@
     <t>-292192</t>
   </si>
   <si>
-    <t>6600</t>
-  </si>
-  <si>
-    <t>11370</t>
-  </si>
-  <si>
-    <t>89380</t>
-  </si>
-  <si>
-    <t>1241677</t>
-  </si>
-  <si>
-    <t>15728295</t>
-  </si>
-  <si>
-    <t>193214564</t>
-  </si>
-  <si>
-    <t>2347661660</t>
-  </si>
-  <si>
-    <t>1630006173</t>
-  </si>
-  <si>
-    <t>300</t>
-  </si>
-  <si>
-    <t>2640</t>
-  </si>
-  <si>
-    <t>41760</t>
-  </si>
-  <si>
-    <t>623520</t>
-  </si>
-  <si>
-    <t>8083560</t>
-  </si>
-  <si>
-    <t>100292040</t>
-  </si>
-  <si>
-    <t>1215908544</t>
-  </si>
-  <si>
-    <t>1259</t>
-  </si>
-  <si>
-    <t>12977</t>
-  </si>
-  <si>
-    <t>228555</t>
-  </si>
-  <si>
-    <t>3569985</t>
-  </si>
-  <si>
-    <t>47375153</t>
-  </si>
-  <si>
-    <t>594394471</t>
-  </si>
-  <si>
-    <t>7273060993</t>
-  </si>
-  <si>
-    <t>7442</t>
-  </si>
-  <si>
-    <t>20222</t>
-  </si>
-  <si>
-    <t>246420</t>
-  </si>
-  <si>
-    <t>3694071</t>
-  </si>
-  <si>
-    <t>48561239</t>
-  </si>
-  <si>
-    <t>606200578</t>
-  </si>
-  <si>
-    <t>7391067132</t>
-  </si>
-  <si>
-    <t>140</t>
-  </si>
-  <si>
-    <t>1364</t>
-  </si>
-  <si>
-    <t>23036</t>
-  </si>
-  <si>
-    <t>354092</t>
-  </si>
-  <si>
-    <t>4650116</t>
-  </si>
-  <si>
-    <t>58175204</t>
-  </si>
-  <si>
-    <t>709545116</t>
-  </si>
-  <si>
-    <t>686</t>
-  </si>
-  <si>
-    <t>6809</t>
-  </si>
-  <si>
-    <t>117537</t>
-  </si>
-  <si>
-    <t>1828655</t>
-  </si>
-  <si>
-    <t>23902863</t>
-  </si>
-  <si>
-    <t>298703551</t>
-  </si>
-  <si>
-    <t>3661896819</t>
-  </si>
-  <si>
-    <t>470000047</t>
-  </si>
-  <si>
-    <t>6869</t>
-  </si>
-  <si>
-    <t>14054</t>
-  </si>
-  <si>
-    <t>135402</t>
-  </si>
-  <si>
-    <t>1952741</t>
-  </si>
-  <si>
-    <t>25088949</t>
-  </si>
-  <si>
-    <t>310509658</t>
-  </si>
-  <si>
-    <t>3779902958</t>
-  </si>
-  <si>
-    <t>1650006175</t>
+    <t>6247</t>
+  </si>
+  <si>
+    <t>11014</t>
+  </si>
+  <si>
+    <t>88126</t>
+  </si>
+  <si>
+    <t>1239613</t>
+  </si>
+  <si>
+    <t>15725826</t>
+  </si>
+  <si>
+    <t>193211555</t>
+  </si>
+  <si>
+    <t>2347658111</t>
+  </si>
+  <si>
+    <t>1630006051</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>2400</t>
+  </si>
+  <si>
+    <t>41160</t>
+  </si>
+  <si>
+    <t>622560</t>
+  </si>
+  <si>
+    <t>8082420</t>
+  </si>
+  <si>
+    <t>100290660</t>
+  </si>
+  <si>
+    <t>1215906924</t>
+  </si>
+  <si>
+    <t>429</t>
+  </si>
+  <si>
+    <t>11930</t>
+  </si>
+  <si>
+    <t>225016</t>
+  </si>
+  <si>
+    <t>3564246</t>
+  </si>
+  <si>
+    <t>47368059</t>
+  </si>
+  <si>
+    <t>594386201</t>
+  </si>
+  <si>
+    <t>7273055453</t>
+  </si>
+  <si>
+    <t>6535</t>
+  </si>
+  <si>
+    <t>19098</t>
+  </si>
+  <si>
+    <t>242804</t>
+  </si>
+  <si>
+    <t>3688255</t>
+  </si>
+  <si>
+    <t>48554068</t>
+  </si>
+  <si>
+    <t>606192231</t>
+  </si>
+  <si>
+    <t>7391061515</t>
+  </si>
+  <si>
+    <t>1240</t>
+  </si>
+  <si>
+    <t>22696</t>
+  </si>
+  <si>
+    <t>353536</t>
+  </si>
+  <si>
+    <t>4649452</t>
+  </si>
+  <si>
+    <t>58174396</t>
+  </si>
+  <si>
+    <t>709544164</t>
+  </si>
+  <si>
+    <t>239</t>
+  </si>
+  <si>
+    <t>6286</t>
+  </si>
+  <si>
+    <t>115678</t>
+  </si>
+  <si>
+    <t>1825610</t>
+  </si>
+  <si>
+    <t>23898884</t>
+  </si>
+  <si>
+    <t>298697314</t>
+  </si>
+  <si>
+    <t>3661899918</t>
+  </si>
+  <si>
+    <t>470000000</t>
+  </si>
+  <si>
+    <t>6345</t>
+  </si>
+  <si>
+    <t>13454</t>
+  </si>
+  <si>
+    <t>133466</t>
+  </si>
+  <si>
+    <t>1949619</t>
+  </si>
+  <si>
+    <t>25084893</t>
+  </si>
+  <si>
+    <t>310503344</t>
+  </si>
+  <si>
+    <t>3779905980</t>
+  </si>
+  <si>
+    <t>1650006051</t>
   </si>
 </sst>
 </file>
@@ -942,25 +936,25 @@
         <v>33</v>
       </c>
       <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>35</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>36</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>37</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>38</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>39</v>
-      </c>
-      <c r="H6" t="s">
-        <v>40</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>
@@ -968,28 +962,28 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
         <v>41</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>44</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>45</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>46</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>47</v>
-      </c>
-      <c r="H7" t="s">
-        <v>48</v>
       </c>
       <c r="I7" t="s">
         <v>10</v>
@@ -997,28 +991,28 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
         <v>49</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>50</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>51</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>52</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>53</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>54</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>55</v>
-      </c>
-      <c r="H8" t="s">
-        <v>56</v>
       </c>
       <c r="I8" t="s">
         <v>10</v>
@@ -1026,28 +1020,28 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
         <v>57</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>58</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>59</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>60</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>61</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>62</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>63</v>
-      </c>
-      <c r="H9" t="s">
-        <v>64</v>
       </c>
       <c r="I9" t="s">
         <v>10</v>
@@ -1183,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I4" t="s">
         <v>10</v>
@@ -1212,7 +1206,7 @@
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I5" t="s">
         <v>10</v>
@@ -1249,36 +1243,36 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
         <v>66</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>67</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>68</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>69</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>70</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>71</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>72</v>
-      </c>
-      <c r="I7" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -1290,16 +1284,16 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" t="s">
         <v>74</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>75</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>76</v>
-      </c>
-      <c r="H8" t="s">
-        <v>77</v>
       </c>
       <c r="I8" t="s">
         <v>10</v>
@@ -1307,31 +1301,31 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" t="s">
         <v>78</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>79</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>80</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>81</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>82</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>83</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>84</v>
-      </c>
-      <c r="I9" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1446,25 +1440,25 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" t="s">
         <v>86</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>87</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>88</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>89</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>90</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>91</v>
-      </c>
-      <c r="H4" t="s">
-        <v>92</v>
       </c>
       <c r="I4" t="s">
         <v>10</v>
@@ -1475,25 +1469,25 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
         <v>86</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>87</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>88</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>89</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>90</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>91</v>
-      </c>
-      <c r="H5" t="s">
-        <v>92</v>
       </c>
       <c r="I5" t="s">
         <v>10</v>
@@ -1530,28 +1524,28 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" t="s">
         <v>93</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>94</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>95</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>96</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>97</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>98</v>
-      </c>
-      <c r="H7" t="s">
-        <v>99</v>
       </c>
       <c r="I7" t="s">
         <v>10</v>
@@ -1559,7 +1553,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -1588,28 +1582,28 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" t="s">
         <v>100</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>101</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>102</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>103</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>104</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>105</v>
-      </c>
-      <c r="H9" t="s">
-        <v>106</v>
       </c>
       <c r="I9" t="s">
         <v>10</v>
@@ -1728,25 +1722,25 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" t="s">
         <v>107</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>108</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>109</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>110</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>111</v>
-      </c>
-      <c r="G4" t="s">
-        <v>112</v>
-      </c>
-      <c r="H4" t="s">
-        <v>113</v>
       </c>
       <c r="I4" t="s">
         <v>10</v>
@@ -1757,25 +1751,25 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" t="s">
         <v>107</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>108</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>109</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>110</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>111</v>
-      </c>
-      <c r="G5" t="s">
-        <v>112</v>
-      </c>
-      <c r="H5" t="s">
-        <v>113</v>
       </c>
       <c r="I5" t="s">
         <v>10</v>
@@ -1812,36 +1806,36 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" t="s">
         <v>114</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>115</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>116</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>117</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>118</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>119</v>
-      </c>
-      <c r="H7" t="s">
-        <v>120</v>
-      </c>
-      <c r="I7" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -1870,31 +1864,31 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" t="s">
         <v>122</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>123</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>124</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>125</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>126</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>127</v>
-      </c>
-      <c r="H9" t="s">
-        <v>128</v>
-      </c>
-      <c r="I9" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>